<commit_message>
updates in topic 2 and 3
</commit_message>
<xml_diff>
--- a/topic_2_img/example_lease.xlsx
+++ b/topic_2_img/example_lease.xlsx
@@ -20,11 +20,38 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t xml:space="preserve">Interest rate</t>
   </si>
   <si>
+    <t xml:space="preserve">Operating L.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Capital L.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Liability</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Asset</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(A)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(b1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(b2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(B=b1+b2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(B/A)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Year</t>
   </si>
   <si>
@@ -40,13 +67,16 @@
     <t xml:space="preserve">Interest</t>
   </si>
   <si>
-    <t xml:space="preserve">Lease Obligation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lease Balance</t>
+    <t xml:space="preserve">Lease reduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lease liability</t>
   </si>
   <si>
     <t xml:space="preserve">Depreciation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ROU asset</t>
   </si>
   <si>
     <t xml:space="preserve">Total Expense</t>
@@ -80,7 +110,7 @@
     <numFmt numFmtId="169" formatCode="General"/>
     <numFmt numFmtId="170" formatCode="#,##0"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -103,12 +133,19 @@
       <family val="0"/>
     </font>
     <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <sz val="12"/>
       <name val="Times New Roman"/>
-      <family val="1"/>
+      <family val="0"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -117,12 +154,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor rgb="FFFFFF00"/>
+        <fgColor rgb="FFFFDBB6"/>
+        <bgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFB66C"/>
+        <bgColor rgb="FFFFDBB6"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="15">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -131,10 +174,101 @@
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="thin"/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right style="thin"/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right/>
+      <top/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="thin"/>
+      <top/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right style="thin"/>
+      <top/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right/>
+      <top style="thin"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right/>
+      <top style="thin"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -163,7 +297,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="57">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -172,63 +306,223 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="169" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="3" borderId="10" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="3" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -241,6 +535,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFFB66C"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFDBB6"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -255,19 +609,19 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>742320</xdr:colOff>
+      <xdr:colOff>252000</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>39960</xdr:rowOff>
+      <xdr:rowOff>39600</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
         <xdr:cNvPr id="0" name="Text Frame 1"/>
-        <xdr:cNvSpPr txBox="1"/>
+        <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
           <a:off x="813240" y="3957120"/>
-          <a:ext cx="6011280" cy="1747080"/>
+          <a:ext cx="6010920" cy="1746720"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -277,11 +631,22 @@
           <a:noFill/>
         </a:ln>
       </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
       <xdr:txBody>
         <a:bodyPr lIns="0" rIns="0" tIns="0" bIns="0" anchor="t">
           <a:noAutofit/>
         </a:bodyPr>
         <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
           <a:r>
             <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
               <a:latin typeface="Times New Roman"/>
@@ -293,6 +658,11 @@
           </a:endParaRPr>
         </a:p>
         <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
           <a:r>
             <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
               <a:latin typeface="Times New Roman"/>
@@ -304,17 +674,27 @@
           </a:endParaRPr>
         </a:p>
         <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
           <a:r>
             <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
               <a:latin typeface="Times New Roman"/>
             </a:rPr>
-            <a:t>2. Converting MLP into a liability with two components: (1) interest + (2) capital amortization (as it would be a normal credit liability). Here we keep the lease jergoen an call it “Lease Obligation”.</a:t>
+            <a:t>2. Converting MLP into a liability with two components: (1) interest + (2) capital amortization (as it would be a normal credit liability). Here, we keep the lease jargon and call it “Lease reduction”.</a:t>
           </a:r>
           <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
             <a:latin typeface="Times New Roman"/>
           </a:endParaRPr>
         </a:p>
         <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
           <a:r>
             <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
               <a:latin typeface="Times New Roman"/>
@@ -326,17 +706,27 @@
           </a:endParaRPr>
         </a:p>
         <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
           <a:r>
             <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
               <a:latin typeface="Times New Roman"/>
             </a:rPr>
-            <a:t>For simplicity, we assume that its value equals the PV of the MLP (liability). With this we can compute depreciation expense of the respective assets.</a:t>
+            <a:t>For simplicity, we assume that its value equals the PV of the MLP (liability). With this, we can compute the depreciation expense of the respective asset.</a:t>
           </a:r>
           <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
             <a:latin typeface="Times New Roman"/>
           </a:endParaRPr>
         </a:p>
         <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
           <a:r>
             <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
               <a:latin typeface="Times New Roman"/>
@@ -348,6 +738,11 @@
           </a:endParaRPr>
         </a:p>
         <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
           <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
             <a:latin typeface="Times New Roman"/>
           </a:endParaRPr>
@@ -470,528 +865,630 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B1:K19"/>
+  <dimension ref="B1:M22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O13" activeCellId="0" sqref="O13"/>
+      <selection pane="topLeft" activeCell="L24" activeCellId="0" sqref="L24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="18.05"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="6.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="5.07"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="8.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="7.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="7" style="1" width="12.03"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="13.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="10" style="1" width="13.18"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="n">
+      <c r="C1" s="3" t="n">
         <v>0.0364</v>
       </c>
-      <c r="K1" s="3"/>
+      <c r="L1" s="1"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="3"/>
       <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="4"/>
-    </row>
-    <row r="3" customFormat="false" ht="23.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L2" s="1"/>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="4"/>
+      <c r="D3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="2"/>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="6"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="1"/>
+    </row>
+    <row r="5" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="9"/>
+      <c r="C5" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="D5" s="9"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="G5" s="11"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="I3" s="4" t="s">
+      <c r="J5" s="10"/>
+      <c r="K5" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="J3" s="4" t="s">
+      <c r="L5" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="K3" s="4" t="s">
+      <c r="M5" s="0"/>
+    </row>
+    <row r="6" customFormat="false" ht="23.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="15" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="6" t="n">
+      <c r="C6" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="H6" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="I6" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="J6" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="K6" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="L6" s="21" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="22" t="n">
         <v>2022</v>
       </c>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="7" t="n">
-        <f aca="false">+E14</f>
+      <c r="C7" s="23"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="26"/>
+      <c r="G7" s="25"/>
+      <c r="H7" s="27" t="n">
+        <f aca="false">+E17</f>
         <v>505.254501976769</v>
       </c>
-      <c r="I4" s="6"/>
-      <c r="J4" s="6"/>
-      <c r="K4" s="6"/>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="6" t="n">
-        <f aca="false">+B4+1</f>
+      <c r="I7" s="26"/>
+      <c r="J7" s="28" t="n">
+        <f aca="false">H7</f>
+        <v>505.254501976769</v>
+      </c>
+      <c r="K7" s="25"/>
+      <c r="L7" s="29"/>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="22" t="n">
+        <f aca="false">+B7+1</f>
         <v>2023</v>
       </c>
-      <c r="C5" s="7" t="n">
+      <c r="C8" s="30" t="n">
         <v>124</v>
       </c>
-      <c r="D5" s="8" t="n">
-        <f aca="false">1/(1+$C$1)^(B5-$B$4)</f>
+      <c r="D8" s="31" t="n">
+        <f aca="false">1/(1+$C$1)^(B8-$B$7)</f>
         <v>0.96487842531841</v>
       </c>
-      <c r="E5" s="7" t="n">
-        <f aca="false">D5*C5</f>
+      <c r="E8" s="32" t="n">
+        <f aca="false">D8*C8</f>
         <v>119.644924739483</v>
       </c>
-      <c r="F5" s="7" t="n">
-        <f aca="false">H4*$C$1</f>
+      <c r="F8" s="28" t="n">
+        <f aca="false">H7*$C$1</f>
         <v>18.3912638719544</v>
       </c>
-      <c r="G5" s="7" t="n">
-        <f aca="false">+C5-F5</f>
+      <c r="G8" s="32" t="n">
+        <f aca="false">+C8-F8</f>
         <v>105.608736128046</v>
       </c>
-      <c r="H5" s="7" t="n">
-        <f aca="false">+H4-G5</f>
+      <c r="H8" s="27" t="n">
+        <f aca="false">+H7-G8</f>
         <v>399.645765848724</v>
       </c>
-      <c r="I5" s="7" t="n">
-        <f aca="false">$H$4/($B$13-$B$4)</f>
+      <c r="I8" s="28" t="n">
+        <f aca="false">$H$7/($B$16-$B$7)</f>
         <v>56.1393891085299</v>
       </c>
-      <c r="J5" s="7" t="n">
-        <f aca="false">+I5+F5</f>
-        <v>74.5306529804844</v>
-      </c>
-      <c r="K5" s="9" t="n">
-        <f aca="false">J5/C5</f>
-        <v>0.601053653068423</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="6" t="n">
-        <f aca="false">+B5+1</f>
+      <c r="J8" s="28" t="n">
+        <f aca="false">J7-I8</f>
+        <v>449.115112868239</v>
+      </c>
+      <c r="K8" s="32" t="n">
+        <f aca="false">+I8+F8</f>
+        <v>74.5306529804843</v>
+      </c>
+      <c r="L8" s="33" t="n">
+        <f aca="false">K8/C8</f>
+        <v>0.601053653068422</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="22" t="n">
+        <f aca="false">+B8+1</f>
         <v>2024</v>
       </c>
-      <c r="C6" s="7" t="n">
+      <c r="C9" s="30" t="n">
         <v>88</v>
       </c>
-      <c r="D6" s="8" t="n">
-        <f aca="false">1/(1+$C$1)^(B6-$B$4)</f>
+      <c r="D9" s="31" t="n">
+        <f aca="false">1/(1+$C$1)^(B9-$B$7)</f>
         <v>0.930990375644934</v>
       </c>
-      <c r="E6" s="7" t="n">
-        <f aca="false">D6*C6</f>
+      <c r="E9" s="32" t="n">
+        <f aca="false">D9*C9</f>
         <v>81.9271530567542</v>
       </c>
-      <c r="F6" s="7" t="n">
-        <f aca="false">H5*$C$1</f>
+      <c r="F9" s="28" t="n">
+        <f aca="false">H8*$C$1</f>
         <v>14.5471058768935</v>
       </c>
-      <c r="G6" s="7" t="n">
-        <f aca="false">+C6-F6</f>
+      <c r="G9" s="32" t="n">
+        <f aca="false">+C9-F9</f>
         <v>73.4528941231065</v>
       </c>
-      <c r="H6" s="7" t="n">
-        <f aca="false">+H5-G6</f>
+      <c r="H9" s="27" t="n">
+        <f aca="false">+H8-G9</f>
         <v>326.192871725617</v>
       </c>
-      <c r="I6" s="7" t="n">
-        <f aca="false">$H$4/($B$13-$B$4)</f>
+      <c r="I9" s="28" t="n">
+        <f aca="false">$H$7/($B$16-$B$7)</f>
         <v>56.1393891085299</v>
       </c>
-      <c r="J6" s="7" t="n">
-        <f aca="false">+I6+F6</f>
+      <c r="J9" s="28" t="n">
+        <f aca="false">J8-I9</f>
+        <v>392.975723759709</v>
+      </c>
+      <c r="K9" s="32" t="n">
+        <f aca="false">+I9+F9</f>
         <v>70.6864949854235</v>
       </c>
-      <c r="K6" s="9" t="n">
-        <f aca="false">J6/C6</f>
+      <c r="L9" s="33" t="n">
+        <f aca="false">K9/C9</f>
         <v>0.803255624834358</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="6" t="n">
-        <f aca="false">+B6+1</f>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="22" t="n">
+        <f aca="false">+B9+1</f>
         <v>2025</v>
       </c>
-      <c r="C7" s="7" t="n">
+      <c r="C10" s="30" t="n">
         <v>69</v>
       </c>
-      <c r="D7" s="8" t="n">
-        <f aca="false">1/(1+$C$1)^(B7-$B$4)</f>
+      <c r="D10" s="31" t="n">
+        <f aca="false">1/(1+$C$1)^(B10-$B$7)</f>
         <v>0.898292527638879</v>
       </c>
-      <c r="E7" s="7" t="n">
-        <f aca="false">D7*C7</f>
+      <c r="E10" s="32" t="n">
+        <f aca="false">D10*C10</f>
         <v>61.9821844070827</v>
       </c>
-      <c r="F7" s="7" t="n">
-        <f aca="false">H6*$C$1</f>
+      <c r="F10" s="28" t="n">
+        <f aca="false">H9*$C$1</f>
         <v>11.8734205308125</v>
       </c>
-      <c r="G7" s="7" t="n">
-        <f aca="false">+C7-F7</f>
+      <c r="G10" s="32" t="n">
+        <f aca="false">+C10-F10</f>
         <v>57.1265794691875</v>
       </c>
-      <c r="H7" s="7" t="n">
-        <f aca="false">+H6-G7</f>
+      <c r="H10" s="27" t="n">
+        <f aca="false">+H9-G10</f>
         <v>269.06629225643</v>
       </c>
-      <c r="I7" s="7" t="n">
-        <f aca="false">$H$4/($B$13-$B$4)</f>
+      <c r="I10" s="28" t="n">
+        <f aca="false">$H$7/($B$16-$B$7)</f>
         <v>56.1393891085299</v>
       </c>
-      <c r="J7" s="7" t="n">
-        <f aca="false">+I7+F7</f>
+      <c r="J10" s="28" t="n">
+        <f aca="false">J9-I10</f>
+        <v>336.83633465118</v>
+      </c>
+      <c r="K10" s="32" t="n">
+        <f aca="false">+I10+F10</f>
         <v>68.0128096393424</v>
       </c>
-      <c r="K7" s="9" t="n">
-        <f aca="false">J7/C7</f>
+      <c r="L10" s="33" t="n">
+        <f aca="false">K10/C10</f>
         <v>0.985692893323803</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="6" t="n">
-        <f aca="false">+B7+1</f>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B11" s="22" t="n">
+        <f aca="false">+B10+1</f>
         <v>2026</v>
       </c>
-      <c r="C8" s="7" t="n">
+      <c r="C11" s="30" t="n">
         <v>54</v>
       </c>
-      <c r="D8" s="8" t="n">
-        <f aca="false">1/(1+$C$1)^(B8-$B$4)</f>
+      <c r="D11" s="31" t="n">
+        <f aca="false">1/(1+$C$1)^(B11-$B$7)</f>
         <v>0.866743079543496</v>
       </c>
-      <c r="E8" s="7" t="n">
-        <f aca="false">D8*C8</f>
+      <c r="E11" s="32" t="n">
+        <f aca="false">D11*C11</f>
         <v>46.8041262953488</v>
       </c>
-      <c r="F8" s="7" t="n">
-        <f aca="false">H7*$C$1</f>
-        <v>9.79401303813405</v>
-      </c>
-      <c r="G8" s="7" t="n">
-        <f aca="false">+C8-F8</f>
+      <c r="F11" s="28" t="n">
+        <f aca="false">H10*$C$1</f>
+        <v>9.79401303813404</v>
+      </c>
+      <c r="G11" s="32" t="n">
+        <f aca="false">+C11-F11</f>
         <v>44.205986961866</v>
       </c>
-      <c r="H8" s="7" t="n">
-        <f aca="false">+H7-G8</f>
+      <c r="H11" s="27" t="n">
+        <f aca="false">+H10-G11</f>
         <v>224.860305294564</v>
       </c>
-      <c r="I8" s="7" t="n">
-        <f aca="false">$H$4/($B$13-$B$4)</f>
+      <c r="I11" s="28" t="n">
+        <f aca="false">$H$7/($B$16-$B$7)</f>
         <v>56.1393891085299</v>
       </c>
-      <c r="J8" s="7" t="n">
-        <f aca="false">+I8+F8</f>
+      <c r="J11" s="28" t="n">
+        <f aca="false">J10-I11</f>
+        <v>280.69694554265</v>
+      </c>
+      <c r="K11" s="32" t="n">
+        <f aca="false">+I11+F11</f>
         <v>65.933402146664</v>
       </c>
-      <c r="K8" s="9" t="n">
-        <f aca="false">J8/C8</f>
+      <c r="L11" s="33" t="n">
+        <f aca="false">K11/C11</f>
         <v>1.22098892864193</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="6" t="n">
-        <f aca="false">+B8+1</f>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B12" s="22" t="n">
+        <f aca="false">+B11+1</f>
         <v>2027</v>
       </c>
-      <c r="C9" s="7" t="n">
+      <c r="C12" s="30" t="n">
         <v>50</v>
       </c>
-      <c r="D9" s="8" t="n">
-        <f aca="false">1/(1+$C$1)^(B9-$B$4)</f>
+      <c r="D12" s="31" t="n">
+        <f aca="false">1/(1+$C$1)^(B12-$B$7)</f>
         <v>0.836301697745558</v>
       </c>
-      <c r="E9" s="7" t="n">
-        <f aca="false">D9*C9</f>
+      <c r="E12" s="32" t="n">
+        <f aca="false">D12*C12</f>
         <v>41.8150848872779</v>
       </c>
-      <c r="F9" s="7" t="n">
-        <f aca="false">H8*$C$1</f>
-        <v>8.18491511272213</v>
-      </c>
-      <c r="G9" s="7" t="n">
-        <f aca="false">+C9-F9</f>
+      <c r="F12" s="28" t="n">
+        <f aca="false">H11*$C$1</f>
+        <v>8.18491511272212</v>
+      </c>
+      <c r="G12" s="32" t="n">
+        <f aca="false">+C12-F12</f>
         <v>41.8150848872779</v>
       </c>
-      <c r="H9" s="7" t="n">
-        <f aca="false">+H8-G9</f>
+      <c r="H12" s="27" t="n">
+        <f aca="false">+H11-G12</f>
         <v>183.045220407286</v>
       </c>
-      <c r="I9" s="7" t="n">
-        <f aca="false">$H$4/($B$13-$B$4)</f>
+      <c r="I12" s="28" t="n">
+        <f aca="false">$H$7/($B$16-$B$7)</f>
         <v>56.1393891085299</v>
       </c>
-      <c r="J9" s="7" t="n">
-        <f aca="false">+I9+F9</f>
+      <c r="J12" s="28" t="n">
+        <f aca="false">J11-I12</f>
+        <v>224.55755643412</v>
+      </c>
+      <c r="K12" s="32" t="n">
+        <f aca="false">+I12+F12</f>
         <v>64.3243042212521</v>
       </c>
-      <c r="K9" s="9" t="n">
-        <f aca="false">J9/C9</f>
+      <c r="L12" s="33" t="n">
+        <f aca="false">K12/C12</f>
         <v>1.28648608442504</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="6" t="n">
-        <f aca="false">+B9+1</f>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="22" t="n">
+        <f aca="false">+B12+1</f>
         <v>2028</v>
       </c>
-      <c r="C10" s="7" t="n">
+      <c r="C13" s="30" t="n">
         <v>50</v>
       </c>
-      <c r="D10" s="8" t="n">
-        <f aca="false">1/(1+$C$1)^(B10-$B$4)</f>
+      <c r="D13" s="31" t="n">
+        <f aca="false">1/(1+$C$1)^(B13-$B$7)</f>
         <v>0.806929465211846</v>
       </c>
-      <c r="E10" s="7" t="n">
-        <f aca="false">D10*C10</f>
+      <c r="E13" s="32" t="n">
+        <f aca="false">D13*C13</f>
         <v>40.3464732605923</v>
       </c>
-      <c r="F10" s="7" t="n">
-        <f aca="false">H9*$C$1</f>
+      <c r="F13" s="28" t="n">
+        <f aca="false">H12*$C$1</f>
         <v>6.66284602282521</v>
       </c>
-      <c r="G10" s="7" t="n">
-        <f aca="false">+C10-F10</f>
+      <c r="G13" s="32" t="n">
+        <f aca="false">+C13-F13</f>
         <v>43.3371539771748</v>
       </c>
-      <c r="H10" s="7" t="n">
-        <f aca="false">+H9-G10</f>
+      <c r="H13" s="27" t="n">
+        <f aca="false">+H12-G13</f>
         <v>139.708066430111</v>
       </c>
-      <c r="I10" s="7" t="n">
-        <f aca="false">$H$4/($B$13-$B$4)</f>
+      <c r="I13" s="28" t="n">
+        <f aca="false">$H$7/($B$16-$B$7)</f>
         <v>56.1393891085299</v>
       </c>
-      <c r="J10" s="7" t="n">
-        <f aca="false">+I10+F10</f>
-        <v>62.8022351313552</v>
-      </c>
-      <c r="K10" s="9" t="n">
-        <f aca="false">J10/C10</f>
+      <c r="J13" s="28" t="n">
+        <f aca="false">J12-I13</f>
+        <v>168.41816732559</v>
+      </c>
+      <c r="K13" s="32" t="n">
+        <f aca="false">+I13+F13</f>
+        <v>62.8022351313551</v>
+      </c>
+      <c r="L13" s="33" t="n">
+        <f aca="false">K13/C13</f>
         <v>1.2560447026271</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="6" t="n">
-        <f aca="false">+B10+1</f>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B14" s="22" t="n">
+        <f aca="false">+B13+1</f>
         <v>2029</v>
       </c>
-      <c r="C11" s="7" t="n">
+      <c r="C14" s="30" t="n">
         <v>50</v>
       </c>
-      <c r="D11" s="8" t="n">
-        <f aca="false">1/(1+$C$1)^(B11-$B$4)</f>
+      <c r="D14" s="31" t="n">
+        <f aca="false">1/(1+$C$1)^(B14-$B$7)</f>
         <v>0.778588831736633</v>
       </c>
-      <c r="E11" s="7" t="n">
-        <f aca="false">D11*C11</f>
+      <c r="E14" s="32" t="n">
+        <f aca="false">D14*C14</f>
         <v>38.9294415868317</v>
       </c>
-      <c r="F11" s="7" t="n">
-        <f aca="false">H10*$C$1</f>
-        <v>5.08537361805605</v>
-      </c>
-      <c r="G11" s="7" t="n">
-        <f aca="false">+C11-F11</f>
+      <c r="F14" s="28" t="n">
+        <f aca="false">H13*$C$1</f>
+        <v>5.08537361805604</v>
+      </c>
+      <c r="G14" s="32" t="n">
+        <f aca="false">+C14-F14</f>
         <v>44.914626381944</v>
       </c>
-      <c r="H11" s="7" t="n">
-        <f aca="false">+H10-G11</f>
-        <v>94.7934400481674</v>
-      </c>
-      <c r="I11" s="7" t="n">
-        <f aca="false">$H$4/($B$13-$B$4)</f>
+      <c r="H14" s="27" t="n">
+        <f aca="false">+H13-G14</f>
+        <v>94.7934400481672</v>
+      </c>
+      <c r="I14" s="28" t="n">
+        <f aca="false">$H$7/($B$16-$B$7)</f>
         <v>56.1393891085299</v>
       </c>
-      <c r="J11" s="7" t="n">
-        <f aca="false">+I11+F11</f>
+      <c r="J14" s="28" t="n">
+        <f aca="false">J13-I14</f>
+        <v>112.27877821706</v>
+      </c>
+      <c r="K14" s="32" t="n">
+        <f aca="false">+I14+F14</f>
         <v>61.224762726586</v>
       </c>
-      <c r="K11" s="9" t="n">
-        <f aca="false">J11/C11</f>
+      <c r="L14" s="33" t="n">
+        <f aca="false">K14/C14</f>
         <v>1.22449525453172</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="6" t="n">
-        <f aca="false">+B11+1</f>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="22" t="n">
+        <f aca="false">+B14+1</f>
         <v>2030</v>
       </c>
-      <c r="C12" s="7" t="n">
+      <c r="C15" s="30" t="n">
         <v>50</v>
       </c>
-      <c r="D12" s="8" t="n">
-        <f aca="false">1/(1+$C$1)^(B12-$B$4)</f>
+      <c r="D15" s="31" t="n">
+        <f aca="false">1/(1+$C$1)^(B15-$B$7)</f>
         <v>0.751243565936543</v>
       </c>
-      <c r="E12" s="7" t="n">
-        <f aca="false">D12*C12</f>
+      <c r="E15" s="32" t="n">
+        <f aca="false">D15*C15</f>
         <v>37.5621782968271</v>
       </c>
-      <c r="F12" s="7" t="n">
-        <f aca="false">H11*$C$1</f>
-        <v>3.45048121775329</v>
-      </c>
-      <c r="G12" s="7" t="n">
-        <f aca="false">+C12-F12</f>
+      <c r="F15" s="28" t="n">
+        <f aca="false">H14*$C$1</f>
+        <v>3.45048121775328</v>
+      </c>
+      <c r="G15" s="32" t="n">
+        <f aca="false">+C15-F15</f>
         <v>46.5495187822467</v>
       </c>
-      <c r="H12" s="7" t="n">
-        <f aca="false">+H11-G12</f>
-        <v>48.2439212659207</v>
-      </c>
-      <c r="I12" s="7" t="n">
-        <f aca="false">$H$4/($B$13-$B$4)</f>
+      <c r="H15" s="27" t="n">
+        <f aca="false">+H14-G15</f>
+        <v>48.2439212659204</v>
+      </c>
+      <c r="I15" s="28" t="n">
+        <f aca="false">$H$7/($B$16-$B$7)</f>
         <v>56.1393891085299</v>
       </c>
-      <c r="J12" s="7" t="n">
-        <f aca="false">+I12+F12</f>
+      <c r="J15" s="28" t="n">
+        <f aca="false">J14-I15</f>
+        <v>56.1393891085299</v>
+      </c>
+      <c r="K15" s="32" t="n">
+        <f aca="false">+I15+F15</f>
         <v>59.5898703262832</v>
       </c>
-      <c r="K12" s="9" t="n">
-        <f aca="false">J12/C12</f>
+      <c r="L15" s="33" t="n">
+        <f aca="false">K15/C15</f>
         <v>1.19179740652566</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="10" t="n">
-        <f aca="false">+B12+1</f>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B16" s="34" t="n">
+        <f aca="false">+B15+1</f>
         <v>2031</v>
       </c>
-      <c r="C13" s="11" t="n">
+      <c r="C16" s="35" t="n">
         <v>50</v>
       </c>
-      <c r="D13" s="12" t="n">
-        <f aca="false">1/(1+$C$1)^(B13-$B$4)</f>
+      <c r="D16" s="36" t="n">
+        <f aca="false">1/(1+$C$1)^(B16-$B$7)</f>
         <v>0.724858708931438</v>
       </c>
-      <c r="E13" s="11" t="n">
-        <f aca="false">D13*C13</f>
+      <c r="E16" s="37" t="n">
+        <f aca="false">D16*C16</f>
         <v>36.2429354465719</v>
       </c>
-      <c r="F13" s="11" t="n">
-        <f aca="false">H12*$C$1</f>
-        <v>1.75607873407951</v>
-      </c>
-      <c r="G13" s="11" t="n">
-        <f aca="false">+C13-F13</f>
+      <c r="F16" s="38" t="n">
+        <f aca="false">H15*$C$1</f>
+        <v>1.7560787340795</v>
+      </c>
+      <c r="G16" s="37" t="n">
+        <f aca="false">+C16-F16</f>
         <v>48.2439212659205</v>
       </c>
-      <c r="H13" s="11" t="n">
-        <f aca="false">+H12-G13</f>
+      <c r="H16" s="39" t="n">
+        <f aca="false">+H15-G16</f>
         <v>0</v>
       </c>
-      <c r="I13" s="11" t="n">
-        <f aca="false">$H$4/($B$13-$B$4)</f>
+      <c r="I16" s="38" t="n">
+        <f aca="false">$H$7/($B$16-$B$7)</f>
         <v>56.1393891085299</v>
       </c>
-      <c r="J13" s="11" t="n">
-        <f aca="false">+I13+F13</f>
+      <c r="J16" s="38" t="n">
+        <f aca="false">J15-I16</f>
+        <v>0</v>
+      </c>
+      <c r="K16" s="37" t="n">
+        <f aca="false">+I16+F16</f>
         <v>57.8954678426094</v>
       </c>
-      <c r="K13" s="13" t="n">
-        <f aca="false">J13/C13</f>
+      <c r="L16" s="40" t="n">
+        <f aca="false">K16/C16</f>
         <v>1.15790935685219</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="C14" s="14" t="n">
-        <f aca="false">SUM(C5:C13)</f>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B17" s="34" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17" s="35" t="n">
+        <f aca="false">SUM(C8:C16)</f>
         <v>585</v>
       </c>
-      <c r="D14" s="10"/>
-      <c r="E14" s="11" t="n">
-        <f aca="false">SUM(E5:E13)</f>
+      <c r="D17" s="41"/>
+      <c r="E17" s="37" t="n">
+        <f aca="false">SUM(E8:E16)</f>
         <v>505.254501976769</v>
       </c>
-      <c r="F14" s="15" t="n">
-        <f aca="false">+SUM(F5:F13)</f>
-        <v>79.7454980232307</v>
-      </c>
-      <c r="G14" s="10"/>
-      <c r="H14" s="10"/>
-      <c r="I14" s="14" t="n">
-        <f aca="false">+SUM(I5:I13)</f>
+      <c r="F17" s="42" t="n">
+        <f aca="false">+SUM(F8:F16)</f>
+        <v>79.7454980232306</v>
+      </c>
+      <c r="G17" s="43"/>
+      <c r="H17" s="44"/>
+      <c r="I17" s="38" t="n">
+        <f aca="false">+SUM(I8:I16)</f>
         <v>505.254501976769</v>
       </c>
-      <c r="J14" s="14" t="n">
-        <f aca="false">+I14+F14</f>
+      <c r="J17" s="38"/>
+      <c r="K17" s="43" t="n">
+        <f aca="false">+I17+F17</f>
         <v>585</v>
       </c>
-      <c r="K14" s="14"/>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C17" s="16" t="n">
+      <c r="L17" s="45"/>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B20" s="46" t="s">
+        <v>22</v>
+      </c>
+      <c r="C20" s="47" t="n">
         <v>2660</v>
       </c>
-      <c r="E17" s="2" t="n">
-        <f aca="false">(J9-C9)/C17</f>
-        <v>0.00538507677490681</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C18" s="16" t="n">
+      <c r="D20" s="48"/>
+      <c r="E20" s="49" t="n">
+        <f aca="false">(K12-C12)/C20</f>
+        <v>0.00538507677490679</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B21" s="50" t="s">
+        <v>23</v>
+      </c>
+      <c r="C21" s="51" t="n">
         <v>15731</v>
       </c>
-      <c r="E18" s="2" t="n">
-        <f aca="false">I14/C18</f>
+      <c r="E21" s="52" t="n">
+        <f aca="false">I17/C21</f>
         <v>0.0321183969217958</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C19" s="16" t="n">
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B22" s="53" t="s">
+        <v>24</v>
+      </c>
+      <c r="C22" s="54" t="n">
         <v>14925</v>
       </c>
-      <c r="E19" s="2" t="n">
-        <f aca="false">I14/C19</f>
+      <c r="D22" s="55"/>
+      <c r="E22" s="56" t="n">
+        <f aca="false">I17/C22</f>
         <v>0.0338528979548924</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D3:K3"/>
+    <mergeCell ref="D4:H4"/>
+    <mergeCell ref="I4:K4"/>
+  </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>